<commit_message>
Notas AVs Wyden UniRuy 20062025
</commit_message>
<xml_diff>
--- a/05 Others/Arquitetura de Computador AV Media Final Wyden Uniruy 2025_1.xlsx
+++ b/05 Others/Arquitetura de Computador AV Media Final Wyden Uniruy 2025_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heleno\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A53538A-CC94-4CA8-A729-79FCB54C0B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F2CB22-F1D2-45F1-A972-49A98E6FA63D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00CE2D0E-0A12-41EE-A73B-9B255E59C8BB}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$I$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$K$48</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="109">
   <si>
     <t>2025.03.86948-1 </t>
   </si>
@@ -309,9 +309,6 @@
   </si>
   <si>
     <t>Aluno</t>
-  </si>
-  <si>
-    <t>Md</t>
   </si>
   <si>
     <t>2014.51.39012-2 </t>
@@ -343,14 +340,7 @@
   </si>
   <si>
     <t>Trab 
-Peso 3</t>
-  </si>
-  <si>
-    <t>Trab 
 Peso 6</t>
-  </si>
-  <si>
-    <t>SIM</t>
   </si>
   <si>
     <t>Md 
@@ -369,6 +359,26 @@
   <si>
     <t>Turma 
 ARA 0039</t>
+  </si>
+  <si>
+    <t>TRAB</t>
+  </si>
+  <si>
+    <t>Trab 
+Dif Trab 
+AV</t>
+  </si>
+  <si>
+    <t>Md 
+AV</t>
+  </si>
+  <si>
+    <t>SIM 
+1 e 2</t>
+  </si>
+  <si>
+    <t>Md 
+Final OK</t>
   </si>
 </sst>
 </file>
@@ -476,7 +486,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -658,12 +668,73 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -676,11 +747,8 @@
     <xf numFmtId="43" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -720,16 +788,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="5" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="5" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="5" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="5" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -747,6 +808,43 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="6" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="5" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="5" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="5" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1082,30 +1180,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E31D1293-3D8F-42E6-B03F-BD11486ECFC6}">
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="18" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="56.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="35.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="15.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="35.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="18" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="57" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
-        <v>106</v>
+    <row r="1" spans="1:14" ht="57" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="40" t="s">
+        <v>103</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>88</v>
@@ -1113,33 +1215,39 @@
       <c r="C1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="J1" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="H1" s="18" t="s">
+      <c r="K1" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="L1" s="42" t="s">
         <v>100</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="K1" s="27" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="28">
+      <c r="M1" s="24" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="25">
         <v>3005</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1148,113 +1256,132 @@
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="40">
+      <c r="D2" s="30">
         <v>4.2</v>
       </c>
-      <c r="E2" s="22">
+      <c r="E2" s="19">
         <v>4.2</v>
       </c>
       <c r="F2" s="5">
         <f>E2/7*4</f>
         <v>2.4</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="36"/>
+      <c r="H2" s="4">
         <v>4.8</v>
       </c>
-      <c r="H2" s="22">
-        <f>G2/6*3</f>
-        <v>2.4</v>
-      </c>
-      <c r="I2" s="5">
-        <f>E2+H2</f>
-        <v>6.6</v>
-      </c>
-      <c r="J2" s="46"/>
-      <c r="K2" s="37"/>
-    </row>
-    <row r="3" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="29">
+      <c r="I2" s="4">
+        <v>3</v>
+      </c>
+      <c r="J2" s="19">
+        <f>H2-I2</f>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="K2" s="5">
+        <f>F2+J2</f>
+        <v>4.1999999999999993</v>
+      </c>
+      <c r="L2" s="45"/>
+      <c r="M2" s="58">
+        <f>K2+I2</f>
+        <v>7.1999999999999993</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="26">
         <v>3005</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="41">
+      <c r="C3" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="31">
         <v>2.8</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="13">
         <v>3.4</v>
       </c>
       <c r="F3" s="8">
         <f t="shared" ref="F3:F48" si="0">E3/7*4</f>
         <v>1.9428571428571428</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="37">
+        <v>0.8</v>
+      </c>
+      <c r="H3" s="7">
         <v>3.6</v>
       </c>
-      <c r="H3" s="23">
-        <f t="shared" ref="H3:H48" si="1">G3/6*3</f>
-        <v>1.7999999999999998</v>
-      </c>
-      <c r="I3" s="32">
-        <f t="shared" ref="I3:I48" si="2">E3+H3</f>
-        <v>5.1999999999999993</v>
-      </c>
-      <c r="J3" s="47">
-        <v>0.8</v>
-      </c>
-      <c r="K3" s="38">
-        <f>I3+J3</f>
+      <c r="I3" s="7">
+        <v>3</v>
+      </c>
+      <c r="J3" s="19">
+        <f t="shared" ref="J3:J13" si="1">H3-I3</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="K3" s="5">
+        <f t="shared" ref="K3:K13" si="2">F3+J3</f>
+        <v>2.5428571428571427</v>
+      </c>
+      <c r="L3" s="48">
         <v>5.9999999999999991</v>
       </c>
-      <c r="L3" s="17" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="29">
+      <c r="M3" s="61">
+        <f t="shared" ref="M3:M13" si="3">K3+I3</f>
+        <v>5.5428571428571427</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="26">
         <v>3005</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="41">
+      <c r="D4" s="31">
         <v>0.7</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="13">
         <v>2.2999999999999998</v>
       </c>
       <c r="F4" s="8">
         <f t="shared" si="0"/>
         <v>1.3142857142857143</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="37">
+        <v>0.7</v>
+      </c>
+      <c r="H4" s="7">
         <v>6</v>
       </c>
-      <c r="H4" s="23">
+      <c r="I4" s="7">
+        <v>3</v>
+      </c>
+      <c r="J4" s="19">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I4" s="32">
+      <c r="K4" s="5">
         <f t="shared" si="2"/>
-        <v>5.3</v>
-      </c>
-      <c r="J4" s="47">
-        <v>0.7</v>
-      </c>
-      <c r="K4" s="38">
-        <f>I4+J4</f>
+        <v>4.3142857142857141</v>
+      </c>
+      <c r="L4" s="48">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="29">
+      <c r="M4" s="58">
+        <f t="shared" si="3"/>
+        <v>7.3142857142857141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="26">
         <v>3005</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -1263,32 +1390,39 @@
       <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="41">
+      <c r="D5" s="31">
         <v>3.5</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="20">
         <v>3.5</v>
       </c>
       <c r="F5" s="8">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="37"/>
+      <c r="H5" s="7">
         <v>6</v>
       </c>
-      <c r="H5" s="23">
+      <c r="I5" s="7">
+        <v>3</v>
+      </c>
+      <c r="J5" s="19">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I5" s="8">
+      <c r="K5" s="5">
         <f t="shared" si="2"/>
-        <v>6.5</v>
-      </c>
-      <c r="J5" s="47"/>
-      <c r="K5" s="35"/>
-    </row>
-    <row r="6" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="29">
+        <v>5</v>
+      </c>
+      <c r="L5" s="46"/>
+      <c r="M5" s="58">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="26">
         <v>3005</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -1297,32 +1431,39 @@
       <c r="C6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="41">
+      <c r="D6" s="31">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="20">
         <v>4.9000000000000004</v>
       </c>
       <c r="F6" s="8">
         <f t="shared" si="0"/>
         <v>2.8000000000000003</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="37"/>
+      <c r="H6" s="7">
         <v>4.8</v>
       </c>
-      <c r="H6" s="23">
+      <c r="I6" s="7">
+        <v>3</v>
+      </c>
+      <c r="J6" s="19">
         <f t="shared" si="1"/>
-        <v>2.4</v>
-      </c>
-      <c r="I6" s="8">
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="K6" s="5">
         <f t="shared" si="2"/>
-        <v>7.3000000000000007</v>
-      </c>
-      <c r="J6" s="47"/>
-      <c r="K6" s="35"/>
-    </row>
-    <row r="7" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="29">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="L6" s="46"/>
+      <c r="M6" s="58">
+        <f t="shared" si="3"/>
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="26">
         <v>3005</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -1331,29 +1472,35 @@
       <c r="C7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="H7" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="I7" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="J7" s="47"/>
-      <c r="K7" s="35"/>
-    </row>
-    <row r="8" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="29">
+      <c r="D7" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" s="37"/>
+      <c r="H7" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="J7" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="K7" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="L7" s="47"/>
+      <c r="M7" s="59" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="26">
         <v>3005</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -1362,32 +1509,39 @@
       <c r="C8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="41">
+      <c r="D8" s="31">
         <v>4.2</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="20">
         <v>4.2</v>
       </c>
       <c r="F8" s="8">
         <f t="shared" si="0"/>
         <v>2.4</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="37"/>
+      <c r="H8" s="7">
         <v>4.5</v>
       </c>
-      <c r="H8" s="23">
+      <c r="I8" s="7">
+        <v>3</v>
+      </c>
+      <c r="J8" s="19">
         <f t="shared" si="1"/>
-        <v>2.25</v>
-      </c>
-      <c r="I8" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="K8" s="5">
         <f t="shared" si="2"/>
-        <v>6.45</v>
-      </c>
-      <c r="J8" s="47"/>
-      <c r="K8" s="35"/>
-    </row>
-    <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="29">
+        <v>3.9</v>
+      </c>
+      <c r="L8" s="46"/>
+      <c r="M8" s="58">
+        <f t="shared" si="3"/>
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="26">
         <v>3005</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -1396,32 +1550,39 @@
       <c r="C9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="41">
+      <c r="D9" s="31">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="20">
         <v>4.9000000000000004</v>
       </c>
       <c r="F9" s="8">
         <f t="shared" si="0"/>
         <v>2.8000000000000003</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="37"/>
+      <c r="H9" s="7">
         <v>4.8</v>
       </c>
-      <c r="H9" s="23">
+      <c r="I9" s="7">
+        <v>3</v>
+      </c>
+      <c r="J9" s="19">
         <f t="shared" si="1"/>
-        <v>2.4</v>
-      </c>
-      <c r="I9" s="8">
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="K9" s="5">
         <f t="shared" si="2"/>
-        <v>7.3000000000000007</v>
-      </c>
-      <c r="J9" s="47"/>
-      <c r="K9" s="35"/>
-    </row>
-    <row r="10" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="29">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="L9" s="46"/>
+      <c r="M9" s="58">
+        <f t="shared" si="3"/>
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="26">
         <v>3005</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -1430,32 +1591,39 @@
       <c r="C10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="41">
+      <c r="D10" s="31">
         <v>6.3</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="20">
         <v>6.3</v>
       </c>
       <c r="F10" s="8">
         <f t="shared" si="0"/>
         <v>3.6</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="37"/>
+      <c r="H10" s="7">
         <v>5.8</v>
       </c>
-      <c r="H10" s="23">
+      <c r="I10" s="7">
+        <v>3</v>
+      </c>
+      <c r="J10" s="19">
         <f t="shared" si="1"/>
-        <v>2.9</v>
-      </c>
-      <c r="I10" s="8">
+        <v>2.8</v>
+      </c>
+      <c r="K10" s="5">
         <f t="shared" si="2"/>
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="J10" s="47"/>
-      <c r="K10" s="35"/>
-    </row>
-    <row r="11" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="29">
+        <v>6.4</v>
+      </c>
+      <c r="L10" s="46"/>
+      <c r="M10" s="58">
+        <f t="shared" si="3"/>
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="26">
         <v>3005</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -1464,32 +1632,39 @@
       <c r="C11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="41">
+      <c r="D11" s="31">
         <v>2.8</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="20">
         <v>2.8</v>
       </c>
       <c r="F11" s="8">
         <f t="shared" si="0"/>
         <v>1.5999999999999999</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="37"/>
+      <c r="H11" s="7">
         <v>6</v>
       </c>
-      <c r="H11" s="23">
+      <c r="I11" s="7">
+        <v>3</v>
+      </c>
+      <c r="J11" s="19">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I11" s="8">
+      <c r="K11" s="5">
         <f t="shared" si="2"/>
-        <v>5.8</v>
-      </c>
-      <c r="J11" s="47"/>
-      <c r="K11" s="35"/>
-    </row>
-    <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="29">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="L11" s="46"/>
+      <c r="M11" s="58">
+        <f t="shared" si="3"/>
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="26">
         <v>3005</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -1498,71 +1673,84 @@
       <c r="C12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="41">
+      <c r="D12" s="31">
         <v>3.5</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="20">
         <v>3.5</v>
       </c>
       <c r="F12" s="8">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="37"/>
+      <c r="H12" s="7">
         <v>4.8</v>
       </c>
-      <c r="H12" s="23">
+      <c r="I12" s="7">
+        <v>3</v>
+      </c>
+      <c r="J12" s="19">
         <f t="shared" si="1"/>
-        <v>2.4</v>
-      </c>
-      <c r="I12" s="8">
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="K12" s="5">
         <f t="shared" si="2"/>
-        <v>5.9</v>
-      </c>
-      <c r="J12" s="47"/>
-      <c r="K12" s="35"/>
-    </row>
-    <row r="13" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="29">
+        <v>3.8</v>
+      </c>
+      <c r="L12" s="46"/>
+      <c r="M12" s="58">
+        <f t="shared" si="3"/>
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="26">
         <v>3005</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="41">
+      <c r="D13" s="31">
         <v>0.7</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="13">
         <v>1.7</v>
       </c>
       <c r="F13" s="8">
         <f t="shared" si="0"/>
         <v>0.97142857142857142</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="37">
+        <v>1.4</v>
+      </c>
+      <c r="H13" s="7">
         <v>5.8</v>
       </c>
-      <c r="H13" s="23">
+      <c r="I13" s="7">
+        <v>3</v>
+      </c>
+      <c r="J13" s="19">
         <f t="shared" si="1"/>
-        <v>2.9</v>
-      </c>
-      <c r="I13" s="32">
+        <v>2.8</v>
+      </c>
+      <c r="K13" s="5">
         <f t="shared" si="2"/>
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="J13" s="47">
-        <v>1.4</v>
-      </c>
-      <c r="K13" s="38">
-        <f>I13+J13</f>
+        <v>3.7714285714285714</v>
+      </c>
+      <c r="L13" s="48">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="29">
+      <c r="M13" s="58">
+        <f t="shared" si="3"/>
+        <v>6.7714285714285714</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="26">
         <v>3005</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -1571,65 +1759,82 @@
       <c r="C14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="E14" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="H14" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="I14" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="J14" s="47"/>
-      <c r="K14" s="35"/>
-    </row>
-    <row r="15" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="29">
-        <v>3005</v>
-      </c>
-      <c r="B15" s="49" t="s">
+      <c r="D14" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="G14" s="37"/>
+      <c r="H14" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="J14" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="K14" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="L14" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="M14" s="60" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="26">
+        <v>3005</v>
+      </c>
+      <c r="B15" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="41">
+      <c r="D15" s="31">
         <v>6.3</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="20">
         <v>6.3</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="51">
         <f t="shared" si="0"/>
         <v>3.6</v>
       </c>
-      <c r="G15" s="16">
+      <c r="G15" s="52">
+        <v>0.5</v>
+      </c>
+      <c r="H15" s="13">
         <v>0</v>
       </c>
-      <c r="H15" s="23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="8">
-        <f t="shared" si="2"/>
+      <c r="I15" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="J15" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="K15" s="51">
+        <f>D15</f>
         <v>6.3</v>
       </c>
-      <c r="J15" s="47">
-        <v>0.5</v>
-      </c>
-      <c r="K15" s="35"/>
-    </row>
-    <row r="16" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="29">
+      <c r="L15" s="53">
+        <f>K15</f>
+        <v>6.3</v>
+      </c>
+      <c r="M15" s="54">
+        <f>K15</f>
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="26">
         <v>3005</v>
       </c>
       <c r="B16" s="6" t="s">
@@ -1638,68 +1843,82 @@
       <c r="C16" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="H16" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="I16" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="J16" s="47"/>
-      <c r="K16" s="35"/>
-    </row>
-    <row r="17" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="29">
+      <c r="D16" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="G16" s="37"/>
+      <c r="H16" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="I16" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="J16" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="K16" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="L16" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="M16" s="60" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="26">
         <v>3005</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="C17" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="41">
+      <c r="D17" s="31">
         <v>2.1</v>
       </c>
-      <c r="E17" s="16">
+      <c r="E17" s="13">
         <v>2.8</v>
       </c>
       <c r="F17" s="8">
         <f t="shared" si="0"/>
         <v>1.5999999999999999</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="37">
+        <v>1.3</v>
+      </c>
+      <c r="H17" s="7">
         <v>3.8</v>
       </c>
-      <c r="H17" s="23">
-        <f t="shared" si="1"/>
-        <v>1.9</v>
-      </c>
-      <c r="I17" s="32">
-        <f t="shared" si="2"/>
-        <v>4.6999999999999993</v>
-      </c>
-      <c r="J17" s="47">
-        <v>1.3</v>
-      </c>
-      <c r="K17" s="38">
-        <f>I17+J17</f>
+      <c r="I17" s="7">
+        <v>3</v>
+      </c>
+      <c r="J17" s="19">
+        <f t="shared" ref="J17:J39" si="4">H17-I17</f>
+        <v>0.79999999999999982</v>
+      </c>
+      <c r="K17" s="5">
+        <f t="shared" ref="K17:K39" si="5">F17+J17</f>
+        <v>2.3999999999999995</v>
+      </c>
+      <c r="L17" s="48">
         <v>5.9999999999999991</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="29">
+      <c r="M17" s="61">
+        <f t="shared" ref="M17:M46" si="6">K17+I17</f>
+        <v>5.3999999999999995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="26">
         <v>3005</v>
       </c>
       <c r="B18" s="6" t="s">
@@ -1708,32 +1927,39 @@
       <c r="C18" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="41">
+      <c r="D18" s="31">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E18" s="23">
+      <c r="E18" s="20">
         <v>4.9000000000000004</v>
       </c>
       <c r="F18" s="8">
         <f t="shared" si="0"/>
         <v>2.8000000000000003</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="37"/>
+      <c r="H18" s="7">
         <v>6</v>
       </c>
-      <c r="H18" s="23">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="I18" s="8">
-        <f t="shared" si="2"/>
-        <v>7.9</v>
-      </c>
-      <c r="J18" s="47"/>
-      <c r="K18" s="35"/>
-    </row>
-    <row r="19" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="29">
+      <c r="I18" s="7">
+        <v>3</v>
+      </c>
+      <c r="J18" s="19">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="K18" s="5">
+        <f t="shared" si="5"/>
+        <v>5.8000000000000007</v>
+      </c>
+      <c r="L18" s="46"/>
+      <c r="M18" s="58">
+        <f t="shared" si="6"/>
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="26">
         <v>3005</v>
       </c>
       <c r="B19" s="6" t="s">
@@ -1742,32 +1968,39 @@
       <c r="C19" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="41">
+      <c r="D19" s="31">
         <v>6.3</v>
       </c>
-      <c r="E19" s="23">
+      <c r="E19" s="20">
         <v>6.3</v>
       </c>
       <c r="F19" s="8">
         <f t="shared" si="0"/>
         <v>3.6</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="37"/>
+      <c r="H19" s="7">
         <v>4.5</v>
       </c>
-      <c r="H19" s="23">
-        <f t="shared" si="1"/>
-        <v>2.25</v>
-      </c>
-      <c r="I19" s="8">
-        <f t="shared" si="2"/>
-        <v>8.5500000000000007</v>
-      </c>
-      <c r="J19" s="47"/>
-      <c r="K19" s="35"/>
-    </row>
-    <row r="20" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="29">
+      <c r="I19" s="7">
+        <v>3</v>
+      </c>
+      <c r="J19" s="19">
+        <f t="shared" si="4"/>
+        <v>1.5</v>
+      </c>
+      <c r="K19" s="5">
+        <f t="shared" si="5"/>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="L19" s="46"/>
+      <c r="M19" s="58">
+        <f t="shared" si="6"/>
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="26">
         <v>3005</v>
       </c>
       <c r="B20" s="6" t="s">
@@ -1776,32 +2009,39 @@
       <c r="C20" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="41">
+      <c r="D20" s="31">
         <v>5.6</v>
       </c>
-      <c r="E20" s="23">
+      <c r="E20" s="20">
         <v>5.6</v>
       </c>
       <c r="F20" s="8">
         <f t="shared" si="0"/>
         <v>3.1999999999999997</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="37"/>
+      <c r="H20" s="7">
         <v>6</v>
       </c>
-      <c r="H20" s="23">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="I20" s="8">
-        <f t="shared" si="2"/>
-        <v>8.6</v>
-      </c>
-      <c r="J20" s="47"/>
-      <c r="K20" s="35"/>
-    </row>
-    <row r="21" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="29">
+      <c r="I20" s="7">
+        <v>3</v>
+      </c>
+      <c r="J20" s="19">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="K20" s="5">
+        <f t="shared" si="5"/>
+        <v>6.1999999999999993</v>
+      </c>
+      <c r="L20" s="46"/>
+      <c r="M20" s="58">
+        <f t="shared" si="6"/>
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="26">
         <v>3005</v>
       </c>
       <c r="B21" s="6" t="s">
@@ -1810,71 +2050,84 @@
       <c r="C21" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="41">
+      <c r="D21" s="31">
         <v>3.5</v>
       </c>
-      <c r="E21" s="23">
+      <c r="E21" s="20">
         <v>3.5</v>
       </c>
       <c r="F21" s="8">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="37"/>
+      <c r="H21" s="7">
         <v>4.8</v>
       </c>
-      <c r="H21" s="23">
-        <f t="shared" si="1"/>
-        <v>2.4</v>
-      </c>
-      <c r="I21" s="8">
-        <f t="shared" si="2"/>
-        <v>5.9</v>
-      </c>
-      <c r="J21" s="47"/>
-      <c r="K21" s="35"/>
-    </row>
-    <row r="22" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="29">
-        <v>3005</v>
-      </c>
-      <c r="B22" s="49" t="s">
+      <c r="I21" s="7">
+        <v>3</v>
+      </c>
+      <c r="J21" s="19">
+        <f t="shared" si="4"/>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="K21" s="5">
+        <f t="shared" si="5"/>
+        <v>3.8</v>
+      </c>
+      <c r="L21" s="46"/>
+      <c r="M21" s="58">
+        <f t="shared" si="6"/>
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="26">
+        <v>3005</v>
+      </c>
+      <c r="B22" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="41">
+      <c r="D22" s="31">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E22" s="23">
+      <c r="E22" s="20">
         <v>4.9000000000000004</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F22" s="51">
         <f t="shared" si="0"/>
         <v>2.8000000000000003</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="52">
+        <v>1.4</v>
+      </c>
+      <c r="H22" s="7">
         <v>0</v>
       </c>
-      <c r="H22" s="23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="32">
-        <f t="shared" si="2"/>
+      <c r="I22" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="J22" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="K22" s="51">
+        <f>D22</f>
         <v>4.9000000000000004</v>
       </c>
-      <c r="J22" s="47">
-        <v>1.4</v>
-      </c>
-      <c r="K22" s="38">
-        <f>I22+J22</f>
-        <v>6.3000000000000007</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="29">
+      <c r="L22" s="53">
+        <f>K22</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="M22" s="54">
+        <f>K22</f>
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="26">
         <v>3005</v>
       </c>
       <c r="B23" s="6" t="s">
@@ -1883,32 +2136,39 @@
       <c r="C23" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="41">
+      <c r="D23" s="31">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E23" s="23">
+      <c r="E23" s="20">
         <v>4.9000000000000004</v>
       </c>
       <c r="F23" s="8">
         <f t="shared" si="0"/>
         <v>2.8000000000000003</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="37"/>
+      <c r="H23" s="7">
         <v>4.8</v>
       </c>
-      <c r="H23" s="23">
-        <f t="shared" si="1"/>
-        <v>2.4</v>
-      </c>
-      <c r="I23" s="8">
-        <f t="shared" si="2"/>
-        <v>7.3000000000000007</v>
-      </c>
-      <c r="J23" s="47"/>
-      <c r="K23" s="35"/>
-    </row>
-    <row r="24" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="29">
+      <c r="I23" s="7">
+        <v>3</v>
+      </c>
+      <c r="J23" s="19">
+        <f t="shared" si="4"/>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="K23" s="5">
+        <f t="shared" si="5"/>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="L23" s="46"/>
+      <c r="M23" s="58">
+        <f t="shared" si="6"/>
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="26">
         <v>3005</v>
       </c>
       <c r="B24" s="6" t="s">
@@ -1917,32 +2177,39 @@
       <c r="C24" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="41">
+      <c r="D24" s="31">
         <v>3.5</v>
       </c>
-      <c r="E24" s="23">
+      <c r="E24" s="20">
         <v>3.5</v>
       </c>
       <c r="F24" s="8">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G24" s="37"/>
+      <c r="H24" s="7">
         <v>4.8</v>
       </c>
-      <c r="H24" s="23">
-        <f t="shared" si="1"/>
-        <v>2.4</v>
-      </c>
-      <c r="I24" s="8">
-        <f t="shared" si="2"/>
-        <v>5.9</v>
-      </c>
-      <c r="J24" s="47"/>
-      <c r="K24" s="35"/>
-    </row>
-    <row r="25" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="29">
+      <c r="I24" s="7">
+        <v>3</v>
+      </c>
+      <c r="J24" s="19">
+        <f t="shared" si="4"/>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="K24" s="5">
+        <f t="shared" si="5"/>
+        <v>3.8</v>
+      </c>
+      <c r="L24" s="46"/>
+      <c r="M24" s="58">
+        <f t="shared" si="6"/>
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="26">
         <v>3005</v>
       </c>
       <c r="B25" s="6" t="s">
@@ -1951,32 +2218,39 @@
       <c r="C25" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D25" s="41">
+      <c r="D25" s="31">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E25" s="23">
+      <c r="E25" s="20">
         <v>4.9000000000000004</v>
       </c>
       <c r="F25" s="8">
         <f t="shared" si="0"/>
         <v>2.8000000000000003</v>
       </c>
-      <c r="G25" s="7">
+      <c r="G25" s="37"/>
+      <c r="H25" s="7">
         <v>6</v>
       </c>
-      <c r="H25" s="23">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="I25" s="8">
-        <f t="shared" si="2"/>
-        <v>7.9</v>
-      </c>
-      <c r="J25" s="47"/>
-      <c r="K25" s="35"/>
-    </row>
-    <row r="26" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="29">
+      <c r="I25" s="7">
+        <v>3</v>
+      </c>
+      <c r="J25" s="19">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="K25" s="5">
+        <f t="shared" si="5"/>
+        <v>5.8000000000000007</v>
+      </c>
+      <c r="L25" s="46"/>
+      <c r="M25" s="58">
+        <f t="shared" si="6"/>
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="26">
         <v>3005</v>
       </c>
       <c r="B26" s="6" t="s">
@@ -1985,32 +2259,39 @@
       <c r="C26" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="41">
+      <c r="D26" s="31">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E26" s="23">
+      <c r="E26" s="20">
         <v>4.9000000000000004</v>
       </c>
       <c r="F26" s="8">
         <f t="shared" si="0"/>
         <v>2.8000000000000003</v>
       </c>
-      <c r="G26" s="7">
+      <c r="G26" s="37"/>
+      <c r="H26" s="7">
         <v>4.8</v>
       </c>
-      <c r="H26" s="23">
-        <f t="shared" si="1"/>
-        <v>2.4</v>
-      </c>
-      <c r="I26" s="8">
-        <f t="shared" si="2"/>
-        <v>7.3000000000000007</v>
-      </c>
-      <c r="J26" s="47"/>
-      <c r="K26" s="35"/>
-    </row>
-    <row r="27" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="29">
+      <c r="I26" s="7">
+        <v>3</v>
+      </c>
+      <c r="J26" s="19">
+        <f t="shared" si="4"/>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="K26" s="5">
+        <f t="shared" si="5"/>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="L26" s="46"/>
+      <c r="M26" s="58">
+        <f t="shared" si="6"/>
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="26">
         <v>3005</v>
       </c>
       <c r="B27" s="6" t="s">
@@ -2019,32 +2300,39 @@
       <c r="C27" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="41">
+      <c r="D27" s="31">
         <v>3.5</v>
       </c>
-      <c r="E27" s="23">
+      <c r="E27" s="20">
         <v>3.5</v>
       </c>
       <c r="F27" s="8">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="37"/>
+      <c r="H27" s="7">
         <v>6</v>
       </c>
-      <c r="H27" s="23">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="I27" s="8">
-        <f t="shared" si="2"/>
-        <v>6.5</v>
-      </c>
-      <c r="J27" s="47"/>
-      <c r="K27" s="35"/>
-    </row>
-    <row r="28" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="29">
+      <c r="I27" s="7">
+        <v>3</v>
+      </c>
+      <c r="J27" s="19">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="K27" s="5">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="L27" s="46"/>
+      <c r="M27" s="58">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="26">
         <v>3005</v>
       </c>
       <c r="B28" s="6" t="s">
@@ -2053,71 +2341,84 @@
       <c r="C28" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="41">
+      <c r="D28" s="31">
         <v>6.3</v>
       </c>
-      <c r="E28" s="23">
+      <c r="E28" s="20">
         <v>6.3</v>
       </c>
       <c r="F28" s="8">
         <f t="shared" si="0"/>
         <v>3.6</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G28" s="37"/>
+      <c r="H28" s="7">
         <v>4.5</v>
       </c>
-      <c r="H28" s="23">
-        <f t="shared" si="1"/>
-        <v>2.25</v>
-      </c>
-      <c r="I28" s="8">
-        <f t="shared" si="2"/>
-        <v>8.5500000000000007</v>
-      </c>
-      <c r="J28" s="47"/>
-      <c r="K28" s="35"/>
-    </row>
-    <row r="29" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="29">
+      <c r="I28" s="7">
+        <v>3</v>
+      </c>
+      <c r="J28" s="19">
+        <f t="shared" si="4"/>
+        <v>1.5</v>
+      </c>
+      <c r="K28" s="5">
+        <f t="shared" si="5"/>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="L28" s="46"/>
+      <c r="M28" s="58">
+        <f t="shared" si="6"/>
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="26">
         <v>3005</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="45" t="s">
+      <c r="C29" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="D29" s="41">
+      <c r="D29" s="31">
         <v>2.8</v>
       </c>
-      <c r="E29" s="16">
+      <c r="E29" s="13">
         <v>3</v>
       </c>
       <c r="F29" s="8">
         <f t="shared" si="0"/>
         <v>1.7142857142857142</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G29" s="37">
+        <v>0.7</v>
+      </c>
+      <c r="H29" s="7">
         <v>4.8</v>
       </c>
-      <c r="H29" s="23">
-        <f t="shared" si="1"/>
-        <v>2.4</v>
-      </c>
-      <c r="I29" s="34">
-        <f t="shared" si="2"/>
-        <v>5.4</v>
-      </c>
-      <c r="J29" s="47">
-        <v>0.7</v>
-      </c>
-      <c r="K29" s="38">
-        <f>I29+J29</f>
+      <c r="I29" s="7">
+        <v>3</v>
+      </c>
+      <c r="J29" s="19">
+        <f t="shared" si="4"/>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="K29" s="5">
+        <f t="shared" si="5"/>
+        <v>3.5142857142857142</v>
+      </c>
+      <c r="L29" s="48">
         <v>6.1000000000000005</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="29">
+      <c r="M29" s="58">
+        <f t="shared" si="6"/>
+        <v>6.5142857142857142</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="26">
         <v>3005</v>
       </c>
       <c r="B30" s="6" t="s">
@@ -2126,32 +2427,39 @@
       <c r="C30" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D30" s="41">
+      <c r="D30" s="31">
         <v>4.2</v>
       </c>
-      <c r="E30" s="23">
+      <c r="E30" s="20">
         <v>4.2</v>
       </c>
       <c r="F30" s="8">
         <f t="shared" si="0"/>
         <v>2.4</v>
       </c>
-      <c r="G30" s="7">
+      <c r="G30" s="37"/>
+      <c r="H30" s="7">
         <v>4.5</v>
       </c>
-      <c r="H30" s="23">
-        <f t="shared" si="1"/>
-        <v>2.25</v>
-      </c>
-      <c r="I30" s="8">
-        <f t="shared" si="2"/>
-        <v>6.45</v>
-      </c>
-      <c r="J30" s="47"/>
-      <c r="K30" s="35"/>
-    </row>
-    <row r="31" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="29">
+      <c r="I30" s="7">
+        <v>3</v>
+      </c>
+      <c r="J30" s="19">
+        <f t="shared" si="4"/>
+        <v>1.5</v>
+      </c>
+      <c r="K30" s="5">
+        <f t="shared" si="5"/>
+        <v>3.9</v>
+      </c>
+      <c r="L30" s="46"/>
+      <c r="M30" s="58">
+        <f t="shared" si="6"/>
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="26">
         <v>3005</v>
       </c>
       <c r="B31" s="6" t="s">
@@ -2160,32 +2468,39 @@
       <c r="C31" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D31" s="41">
+      <c r="D31" s="31">
         <v>6.3</v>
       </c>
-      <c r="E31" s="23">
+      <c r="E31" s="20">
         <v>6.3</v>
       </c>
       <c r="F31" s="8">
         <f t="shared" si="0"/>
         <v>3.6</v>
       </c>
-      <c r="G31" s="7">
+      <c r="G31" s="37"/>
+      <c r="H31" s="7">
         <v>4.8</v>
       </c>
-      <c r="H31" s="23">
-        <f t="shared" si="1"/>
-        <v>2.4</v>
-      </c>
-      <c r="I31" s="8">
-        <f t="shared" si="2"/>
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="J31" s="47"/>
-      <c r="K31" s="35"/>
-    </row>
-    <row r="32" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="29">
+      <c r="I31" s="7">
+        <v>3</v>
+      </c>
+      <c r="J31" s="19">
+        <f t="shared" si="4"/>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="K31" s="5">
+        <f t="shared" si="5"/>
+        <v>5.4</v>
+      </c>
+      <c r="L31" s="46"/>
+      <c r="M31" s="58">
+        <f t="shared" si="6"/>
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="26">
         <v>3005</v>
       </c>
       <c r="B32" s="6" t="s">
@@ -2194,32 +2509,39 @@
       <c r="C32" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="41">
+      <c r="D32" s="31">
         <v>5.6</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="20">
         <v>5.6</v>
       </c>
       <c r="F32" s="8">
         <f t="shared" si="0"/>
         <v>3.1999999999999997</v>
       </c>
-      <c r="G32" s="7">
+      <c r="G32" s="37"/>
+      <c r="H32" s="7">
         <v>4.8</v>
       </c>
-      <c r="H32" s="23">
-        <f t="shared" si="1"/>
-        <v>2.4</v>
-      </c>
-      <c r="I32" s="8">
-        <f t="shared" si="2"/>
+      <c r="I32" s="7">
+        <v>3</v>
+      </c>
+      <c r="J32" s="19">
+        <f t="shared" si="4"/>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="K32" s="5">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="L32" s="46"/>
+      <c r="M32" s="58">
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
-      <c r="J32" s="47"/>
-      <c r="K32" s="35"/>
-    </row>
-    <row r="33" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="29">
+    </row>
+    <row r="33" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="26">
         <v>3005</v>
       </c>
       <c r="B33" s="6" t="s">
@@ -2228,32 +2550,39 @@
       <c r="C33" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="41">
+      <c r="D33" s="31">
         <v>4.2</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="20">
         <v>4.2</v>
       </c>
       <c r="F33" s="8">
         <f t="shared" si="0"/>
         <v>2.4</v>
       </c>
-      <c r="G33" s="7">
+      <c r="G33" s="37"/>
+      <c r="H33" s="7">
         <v>6</v>
       </c>
-      <c r="H33" s="23">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="I33" s="8">
-        <f t="shared" si="2"/>
-        <v>7.2</v>
-      </c>
-      <c r="J33" s="47"/>
-      <c r="K33" s="35"/>
-    </row>
-    <row r="34" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="29">
+      <c r="I33" s="7">
+        <v>3</v>
+      </c>
+      <c r="J33" s="19">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="K33" s="5">
+        <f t="shared" si="5"/>
+        <v>5.4</v>
+      </c>
+      <c r="L33" s="46"/>
+      <c r="M33" s="58">
+        <f t="shared" si="6"/>
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="26">
         <v>3005</v>
       </c>
       <c r="B34" s="6" t="s">
@@ -2262,29 +2591,35 @@
       <c r="C34" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="E34" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="F34" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="G34" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="H34" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="I34" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="J34" s="47"/>
-      <c r="K34" s="35"/>
-    </row>
-    <row r="35" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="29">
+      <c r="D34" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="G34" s="37"/>
+      <c r="H34" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="I34" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="J34" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="K34" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="L34" s="47"/>
+      <c r="M34" s="59" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="26">
         <v>3005</v>
       </c>
       <c r="B35" s="6" t="s">
@@ -2293,71 +2628,84 @@
       <c r="C35" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D35" s="41">
+      <c r="D35" s="31">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E35" s="23">
+      <c r="E35" s="20">
         <v>4.9000000000000004</v>
       </c>
       <c r="F35" s="8">
         <f t="shared" si="0"/>
         <v>2.8000000000000003</v>
       </c>
-      <c r="G35" s="7">
+      <c r="G35" s="37"/>
+      <c r="H35" s="7">
         <v>4.8</v>
       </c>
-      <c r="H35" s="23">
-        <f t="shared" si="1"/>
-        <v>2.4</v>
-      </c>
-      <c r="I35" s="8">
-        <f t="shared" si="2"/>
-        <v>7.3000000000000007</v>
-      </c>
-      <c r="J35" s="47"/>
-      <c r="K35" s="35"/>
-    </row>
-    <row r="36" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="29">
+      <c r="I35" s="7">
+        <v>3</v>
+      </c>
+      <c r="J35" s="19">
+        <f t="shared" si="4"/>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="K35" s="5">
+        <f t="shared" si="5"/>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="L35" s="46"/>
+      <c r="M35" s="58">
+        <f t="shared" si="6"/>
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A36" s="26">
         <v>3005</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="45" t="s">
+      <c r="C36" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="D36" s="41">
+      <c r="D36" s="31">
         <v>2.1</v>
       </c>
-      <c r="E36" s="16">
+      <c r="E36" s="13">
         <v>3</v>
       </c>
       <c r="F36" s="8">
         <f t="shared" si="0"/>
         <v>1.7142857142857142</v>
       </c>
-      <c r="G36" s="7">
+      <c r="G36" s="37">
+        <v>0.6</v>
+      </c>
+      <c r="H36" s="7">
         <v>4.8</v>
       </c>
-      <c r="H36" s="23">
-        <f t="shared" si="1"/>
-        <v>2.4</v>
-      </c>
-      <c r="I36" s="32">
-        <f t="shared" si="2"/>
-        <v>5.4</v>
-      </c>
-      <c r="J36" s="47">
-        <v>0.6</v>
-      </c>
-      <c r="K36" s="38">
-        <f>I36+J36</f>
+      <c r="I36" s="7">
+        <v>3</v>
+      </c>
+      <c r="J36" s="19">
+        <f t="shared" si="4"/>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="K36" s="5">
+        <f t="shared" si="5"/>
+        <v>3.5142857142857142</v>
+      </c>
+      <c r="L36" s="48">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="29">
+      <c r="M36" s="58">
+        <f t="shared" si="6"/>
+        <v>6.5142857142857142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="26">
         <v>3005</v>
       </c>
       <c r="B37" s="6" t="s">
@@ -2366,35 +2714,42 @@
       <c r="C37" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="41">
+      <c r="D37" s="31">
         <v>7</v>
       </c>
-      <c r="E37" s="23">
+      <c r="E37" s="20">
         <v>7</v>
       </c>
       <c r="F37" s="8">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G37" s="7">
+      <c r="G37" s="37"/>
+      <c r="H37" s="7">
         <v>3.6</v>
       </c>
-      <c r="H37" s="23">
-        <f t="shared" si="1"/>
-        <v>1.7999999999999998</v>
-      </c>
-      <c r="I37" s="8">
-        <f t="shared" si="2"/>
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="J37" s="47"/>
-      <c r="K37" s="35"/>
-      <c r="L37" s="17" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="29">
+      <c r="I37" s="7">
+        <v>3</v>
+      </c>
+      <c r="J37" s="19">
+        <f t="shared" si="4"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="K37" s="5">
+        <f t="shared" si="5"/>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="L37" s="46"/>
+      <c r="M37" s="58">
+        <f t="shared" si="6"/>
+        <v>7.6</v>
+      </c>
+      <c r="N37" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A38" s="26">
         <v>3005</v>
       </c>
       <c r="B38" s="6" t="s">
@@ -2403,32 +2758,39 @@
       <c r="C38" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="41">
+      <c r="D38" s="31">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E38" s="23">
+      <c r="E38" s="20">
         <v>4.9000000000000004</v>
       </c>
       <c r="F38" s="8">
         <f t="shared" si="0"/>
         <v>2.8000000000000003</v>
       </c>
-      <c r="G38" s="7">
+      <c r="G38" s="37"/>
+      <c r="H38" s="7">
         <v>4.8</v>
       </c>
-      <c r="H38" s="23">
-        <f t="shared" si="1"/>
-        <v>2.4</v>
-      </c>
-      <c r="I38" s="8">
-        <f t="shared" si="2"/>
-        <v>7.3000000000000007</v>
-      </c>
-      <c r="J38" s="47"/>
-      <c r="K38" s="35"/>
-    </row>
-    <row r="39" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="29">
+      <c r="I38" s="7">
+        <v>3</v>
+      </c>
+      <c r="J38" s="19">
+        <f t="shared" si="4"/>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="K38" s="5">
+        <f t="shared" si="5"/>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="L38" s="46"/>
+      <c r="M38" s="58">
+        <f t="shared" si="6"/>
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="26">
         <v>3005</v>
       </c>
       <c r="B39" s="6" t="s">
@@ -2437,37 +2799,43 @@
       <c r="C39" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D39" s="41">
+      <c r="D39" s="31">
         <v>2.8</v>
       </c>
-      <c r="E39" s="23">
+      <c r="E39" s="20">
         <v>2.8</v>
       </c>
       <c r="F39" s="8">
         <f t="shared" si="0"/>
         <v>1.5999999999999999</v>
       </c>
-      <c r="G39" s="7">
+      <c r="G39" s="37">
+        <v>0.8</v>
+      </c>
+      <c r="H39" s="7">
         <v>5.8</v>
       </c>
-      <c r="H39" s="23">
-        <f t="shared" si="1"/>
-        <v>2.9</v>
-      </c>
-      <c r="I39" s="8">
-        <f t="shared" si="2"/>
-        <v>5.6999999999999993</v>
-      </c>
-      <c r="J39" s="47">
-        <v>0.8</v>
-      </c>
-      <c r="K39" s="38">
-        <f>I39+J39</f>
+      <c r="I39" s="7">
+        <v>3</v>
+      </c>
+      <c r="J39" s="19">
+        <f t="shared" si="4"/>
+        <v>2.8</v>
+      </c>
+      <c r="K39" s="5">
+        <f t="shared" si="5"/>
+        <v>4.3999999999999995</v>
+      </c>
+      <c r="L39" s="48">
         <v>6.4999999999999991</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A40" s="29">
+      <c r="M39" s="58">
+        <f t="shared" si="6"/>
+        <v>7.3999999999999995</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A40" s="26">
         <v>3005</v>
       </c>
       <c r="B40" s="6" t="s">
@@ -2476,29 +2844,35 @@
       <c r="C40" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D40" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="E40" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="F40" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="G40" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="H40" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="I40" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="J40" s="47"/>
-      <c r="K40" s="35"/>
-    </row>
-    <row r="41" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="29">
+      <c r="D40" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="E40" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="G40" s="37"/>
+      <c r="H40" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="I40" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="J40" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="K40" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="L40" s="47"/>
+      <c r="M40" s="59" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A41" s="26">
         <v>3005</v>
       </c>
       <c r="B41" s="6" t="s">
@@ -2507,29 +2881,35 @@
       <c r="C41" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D41" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="E41" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="F41" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="G41" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="H41" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="I41" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="J41" s="47"/>
-      <c r="K41" s="35"/>
-    </row>
-    <row r="42" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="29">
+      <c r="D41" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="E41" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="F41" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="G41" s="37"/>
+      <c r="H41" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="I41" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="J41" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="K41" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="L41" s="47"/>
+      <c r="M41" s="59" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A42" s="26">
         <v>3005</v>
       </c>
       <c r="B42" s="6" t="s">
@@ -2538,32 +2918,39 @@
       <c r="C42" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D42" s="41">
+      <c r="D42" s="31">
         <v>5.6</v>
       </c>
-      <c r="E42" s="23">
+      <c r="E42" s="20">
         <v>5.6</v>
       </c>
       <c r="F42" s="8">
         <f t="shared" si="0"/>
         <v>3.1999999999999997</v>
       </c>
-      <c r="G42" s="7">
+      <c r="G42" s="37"/>
+      <c r="H42" s="7">
         <v>4.5</v>
       </c>
-      <c r="H42" s="23">
-        <f t="shared" si="1"/>
-        <v>2.25</v>
-      </c>
-      <c r="I42" s="8">
-        <f t="shared" si="2"/>
-        <v>7.85</v>
-      </c>
-      <c r="J42" s="47"/>
-      <c r="K42" s="35"/>
-    </row>
-    <row r="43" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A43" s="29">
+      <c r="I42" s="7">
+        <v>3</v>
+      </c>
+      <c r="J42" s="19">
+        <f t="shared" ref="J42:J45" si="7">H42-I42</f>
+        <v>1.5</v>
+      </c>
+      <c r="K42" s="5">
+        <f t="shared" ref="K42:K45" si="8">F42+J42</f>
+        <v>4.6999999999999993</v>
+      </c>
+      <c r="L42" s="46"/>
+      <c r="M42" s="58">
+        <f t="shared" si="6"/>
+        <v>7.6999999999999993</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="26">
         <v>3005</v>
       </c>
       <c r="B43" s="6" t="s">
@@ -2572,37 +2959,43 @@
       <c r="C43" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D43" s="41">
+      <c r="D43" s="31">
         <v>2.8</v>
       </c>
-      <c r="E43" s="23">
+      <c r="E43" s="20">
         <v>2.8</v>
       </c>
       <c r="F43" s="8">
         <f t="shared" si="0"/>
         <v>1.5999999999999999</v>
       </c>
-      <c r="G43" s="7">
+      <c r="G43" s="37">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H43" s="7">
         <v>4.8</v>
       </c>
-      <c r="H43" s="23">
-        <f t="shared" si="1"/>
-        <v>2.4</v>
-      </c>
-      <c r="I43" s="32">
-        <f t="shared" si="2"/>
-        <v>5.1999999999999993</v>
-      </c>
-      <c r="J43" s="47">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="K43" s="38">
-        <f>I43+J43</f>
+      <c r="I43" s="7">
+        <v>3</v>
+      </c>
+      <c r="J43" s="19">
+        <f t="shared" si="7"/>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="K43" s="5">
+        <f t="shared" si="8"/>
+        <v>3.3999999999999995</v>
+      </c>
+      <c r="L43" s="48">
         <v>6.2999999999999989</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="29">
+      <c r="M43" s="58">
+        <f t="shared" si="6"/>
+        <v>6.3999999999999995</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A44" s="26">
         <v>3005</v>
       </c>
       <c r="B44" s="6" t="s">
@@ -2611,32 +3004,39 @@
       <c r="C44" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D44" s="41">
+      <c r="D44" s="31">
         <v>4.2</v>
       </c>
-      <c r="E44" s="23">
+      <c r="E44" s="20">
         <v>4.2</v>
       </c>
       <c r="F44" s="8">
         <f t="shared" si="0"/>
         <v>2.4</v>
       </c>
-      <c r="G44" s="7">
+      <c r="G44" s="37"/>
+      <c r="H44" s="7">
         <v>6</v>
       </c>
-      <c r="H44" s="23">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="I44" s="8">
-        <f t="shared" si="2"/>
-        <v>7.2</v>
-      </c>
-      <c r="J44" s="47"/>
-      <c r="K44" s="35"/>
-    </row>
-    <row r="45" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="29">
+      <c r="I44" s="7">
+        <v>3</v>
+      </c>
+      <c r="J44" s="19">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="K44" s="5">
+        <f t="shared" si="8"/>
+        <v>5.4</v>
+      </c>
+      <c r="L44" s="46"/>
+      <c r="M44" s="58">
+        <f t="shared" si="6"/>
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="26">
         <v>3005</v>
       </c>
       <c r="B45" s="6" t="s">
@@ -2645,136 +3045,160 @@
       <c r="C45" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="D45" s="41">
+      <c r="D45" s="31">
         <v>6.3</v>
       </c>
-      <c r="E45" s="23">
+      <c r="E45" s="20">
         <v>6.3</v>
       </c>
       <c r="F45" s="8">
         <f t="shared" si="0"/>
         <v>3.6</v>
       </c>
-      <c r="G45" s="7">
+      <c r="G45" s="37"/>
+      <c r="H45" s="7">
         <v>5.8</v>
       </c>
-      <c r="H45" s="23">
-        <f t="shared" si="1"/>
-        <v>2.9</v>
-      </c>
-      <c r="I45" s="8">
-        <f t="shared" si="2"/>
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="J45" s="47"/>
-      <c r="K45" s="35"/>
-    </row>
-    <row r="46" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A46" s="29">
+      <c r="I45" s="7">
+        <v>3</v>
+      </c>
+      <c r="J45" s="19">
+        <f t="shared" si="7"/>
+        <v>2.8</v>
+      </c>
+      <c r="K45" s="5">
+        <f t="shared" si="8"/>
+        <v>6.4</v>
+      </c>
+      <c r="L45" s="46"/>
+      <c r="M45" s="58">
+        <f t="shared" si="6"/>
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A46" s="26">
         <v>3001</v>
       </c>
       <c r="B46" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D46" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="F46" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G46" s="37"/>
+      <c r="H46" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="I46" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="J46" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="K46" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="L46" s="47"/>
+      <c r="M46" s="59" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A47" s="26">
+        <v>3001</v>
+      </c>
+      <c r="B47" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="C47" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D46" s="43" t="s">
-        <v>98</v>
-      </c>
-      <c r="E46" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="F46" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="G46" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="H46" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="I46" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="J46" s="47"/>
-      <c r="K46" s="35"/>
-    </row>
-    <row r="47" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A47" s="29">
+      <c r="D47" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="F47" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G47" s="37"/>
+      <c r="H47" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="I47" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="J47" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="K47" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="L47" s="47"/>
+      <c r="M47" s="60" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="27">
         <v>3001</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B48" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="C48" s="55" t="s">
         <v>95</v>
       </c>
-      <c r="D47" s="43" t="s">
-        <v>98</v>
-      </c>
-      <c r="E47" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="F47" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="G47" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="H47" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="I47" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="J47" s="47"/>
-      <c r="K47" s="35"/>
-    </row>
-    <row r="48" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="30">
-        <v>3001</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="D48" s="44">
+      <c r="D48" s="34">
         <v>2.1</v>
       </c>
-      <c r="E48" s="26">
+      <c r="E48" s="23">
         <v>2.1</v>
       </c>
-      <c r="F48" s="11">
+      <c r="F48" s="10">
         <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
-      <c r="G48" s="15">
+      <c r="G48" s="38">
         <v>0</v>
       </c>
-      <c r="H48" s="36">
-        <f t="shared" si="1"/>
+      <c r="H48" s="12">
         <v>0</v>
       </c>
-      <c r="I48" s="11">
-        <f t="shared" si="2"/>
+      <c r="I48" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="J48" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="K48" s="50">
+        <f>D48</f>
         <v>2.1</v>
       </c>
-      <c r="J48" s="48">
-        <v>0</v>
-      </c>
-      <c r="K48" s="39">
-        <f>I48+J48</f>
+      <c r="L48" s="56">
         <v>2.1</v>
       </c>
+      <c r="M48" s="57">
+        <f>K48+G48</f>
+        <v>2.1</v>
+      </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="31"/>
+      <c r="A49" s="28"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I48" xr:uid="{E31D1293-3D8F-42E6-B03F-BD11486ECFC6}"/>
+  <autoFilter ref="A1:K48" xr:uid="{E31D1293-3D8F-42E6-B03F-BD11486ECFC6}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>